<commit_message>
slicing data array when filtering
</commit_message>
<xml_diff>
--- a/storage/app/servers/LeaseWeb_servers_filters_assignment.xlsx
+++ b/storage/app/servers/LeaseWeb_servers_filters_assignment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thiago\Documents\workspace\leaseweb-technical-assessment\storage\servers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thiago\Documents\workspace\leaseweb-technical-assessment\storage\app\servers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5FB86C-C37A-49A6-B03B-BA6EBBB2BC53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1E73CE-95F0-423C-9293-37D3C47C5B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="4980" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="5325" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="385">
   <si>
     <t>Price</t>
   </si>
@@ -1142,6 +1142,48 @@
   </si>
   <si>
     <t>$2361.99</t>
+  </si>
+  <si>
+    <t>Filters</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Range slider</t>
+  </si>
+  <si>
+    <t>0, 250GB, 500GB, 1TB, 2TB, 3TB, 4TB, 8TB, 12TB, 24TB, 48TB, 72TB</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Checkboxes</t>
+  </si>
+  <si>
+    <t>2GB, 4GB, 8GB, 12GB, 16GB, 24GB, 32GB, 48GB, 64GB, 96GB</t>
+  </si>
+  <si>
+    <t>Harddisk type</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>SAS, SATA, SSD</t>
+  </si>
+  <si>
+    <t>Refer to Location list</t>
   </si>
 </sst>
 </file>
@@ -1165,15 +1207,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1181,13 +1229,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1492,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E487"/>
+  <dimension ref="A1:I487"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,9 +1572,12 @@
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1522,8 +1593,13 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1539,8 +1615,17 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1556,8 +1641,17 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1573,8 +1667,17 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1590,8 +1693,17 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1607,8 +1719,17 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1625,7 +1746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1642,7 +1763,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1659,7 +1780,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1676,7 +1797,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1693,7 +1814,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1710,7 +1831,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1727,7 +1848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1744,7 +1865,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1761,7 +1882,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -9786,6 +9907,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
removing the need of slicing data array
</commit_message>
<xml_diff>
--- a/storage/app/servers/LeaseWeb_servers_filters_assignment.xlsx
+++ b/storage/app/servers/LeaseWeb_servers_filters_assignment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\thiago\Documents\workspace\leaseweb-technical-assessment\storage\app\servers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1E73CE-95F0-423C-9293-37D3C47C5B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD9EF0B-F6C2-40F9-9127-CA4C584C4712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5325" yWindow="5325" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2435" uniqueCount="371">
   <si>
     <t>Price</t>
   </si>
@@ -1142,48 +1142,6 @@
   </si>
   <si>
     <t>$2361.99</t>
-  </si>
-  <si>
-    <t>Filters</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>Range slider</t>
-  </si>
-  <si>
-    <t>0, 250GB, 500GB, 1TB, 2TB, 3TB, 4TB, 8TB, 12TB, 24TB, 48TB, 72TB</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>Checkboxes</t>
-  </si>
-  <si>
-    <t>2GB, 4GB, 8GB, 12GB, 16GB, 24GB, 32GB, 48GB, 64GB, 96GB</t>
-  </si>
-  <si>
-    <t>Harddisk type</t>
-  </si>
-  <si>
-    <t>Dropdown</t>
-  </si>
-  <si>
-    <t>SAS, SATA, SSD</t>
-  </si>
-  <si>
-    <t>Refer to Location list</t>
   </si>
 </sst>
 </file>
@@ -1207,21 +1165,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1229,33 +1181,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1560,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I487"/>
+  <dimension ref="A1:E487"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,12 +1504,9 @@
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.7109375" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="57.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1593,13 +1522,8 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1615,17 +1539,8 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1641,17 +1556,8 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1667,17 +1573,8 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1693,17 +1590,8 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1719,17 +1607,8 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1746,7 +1625,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1763,7 +1642,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1780,7 +1659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -1797,7 +1676,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1814,7 +1693,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1831,7 +1710,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1848,7 +1727,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1865,7 +1744,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1882,7 +1761,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -9907,9 +9786,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G1:I1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>